<commit_message>
major code changes.; new outputs and results
</commit_message>
<xml_diff>
--- a/results/control_scenario_sim.xlsx
+++ b/results/control_scenario_sim.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>min load val</t>
   </si>
@@ -22,34 +22,31 @@
     <t>min load time</t>
   </si>
   <si>
-    <t>18:37:00</t>
-  </si>
-  <si>
-    <t>18:49:00</t>
-  </si>
-  <si>
-    <t>21:17:00</t>
-  </si>
-  <si>
-    <t>18:24:00</t>
-  </si>
-  <si>
-    <t>19:45:00</t>
+    <t>18:25:00</t>
+  </si>
+  <si>
+    <t>18:28:00</t>
+  </si>
+  <si>
+    <t>19:28:00</t>
+  </si>
+  <si>
+    <t>18:26:00</t>
+  </si>
+  <si>
+    <t>18:21:00</t>
+  </si>
+  <si>
+    <t>18:33:00</t>
   </si>
   <si>
     <t>18:34:00</t>
   </si>
   <si>
-    <t>18:06:00</t>
-  </si>
-  <si>
-    <t>19:30:00</t>
-  </si>
-  <si>
-    <t>18:36:00</t>
-  </si>
-  <si>
-    <t>20:00:00</t>
+    <t>18:48:00</t>
+  </si>
+  <si>
+    <t>18:16:00</t>
   </si>
 </sst>
 </file>
@@ -426,7 +423,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.03874</v>
+        <v>1.01134</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -437,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.04074</v>
+        <v>1.01456</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -448,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.04106</v>
+        <v>1.01123</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -459,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.03936</v>
+        <v>1.01825</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -470,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.04204</v>
+        <v>1.00783</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -481,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1.04021</v>
+        <v>1.00856</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -492,7 +489,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1.04239</v>
+        <v>1.01328</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -503,7 +500,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.04034</v>
+        <v>1.0012</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -514,10 +511,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.04151</v>
+        <v>1.00574</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -525,10 +522,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.04117</v>
+        <v>1.00806</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>